<commit_message>
Generated final submission values for part 1.1
</commit_message>
<xml_diff>
--- a/data/daniel/output/processed_d.xlsx
+++ b/data/daniel/output/processed_d.xlsx
@@ -460,13 +460,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4.02</v>
+        <v>4.0204</v>
       </c>
       <c r="C2" t="n">
-        <v>4.52</v>
+        <v>4.5157</v>
       </c>
       <c r="D2" t="n">
-        <v>1.61</v>
+        <v>1.6098</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.29</v>
+        <v>3.2872</v>
       </c>
       <c r="C3" t="n">
-        <v>3.88</v>
+        <v>3.8755</v>
       </c>
       <c r="D3" t="n">
-        <v>1.83</v>
+        <v>1.8316</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.4</v>
+        <v>3.4021</v>
       </c>
       <c r="C4" t="n">
-        <v>3.93</v>
+        <v>3.9344</v>
       </c>
       <c r="D4" t="n">
-        <v>1.55</v>
+        <v>1.5457</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.02</v>
+        <v>3.0174</v>
       </c>
       <c r="C5" t="n">
-        <v>3.38</v>
+        <v>3.382</v>
       </c>
       <c r="D5" t="n">
-        <v>1.56</v>
+        <v>1.5601</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.04</v>
+        <v>3.045</v>
       </c>
       <c r="C6" t="n">
-        <v>3.66</v>
+        <v>3.6609</v>
       </c>
       <c r="D6" t="n">
-        <v>1.83</v>
+        <v>1.8298</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.85</v>
+        <v>2.8501</v>
       </c>
       <c r="C7" t="n">
-        <v>3.32</v>
+        <v>3.3194</v>
       </c>
       <c r="D7" t="n">
-        <v>1.53</v>
+        <v>1.5275</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.19</v>
+        <v>3.1895</v>
       </c>
       <c r="C8" t="n">
-        <v>3.47</v>
+        <v>3.4672</v>
       </c>
       <c r="D8" t="n">
-        <v>1.52</v>
+        <v>1.5194</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>2.98</v>
+        <v>2.9765</v>
       </c>
       <c r="C9" t="n">
-        <v>3.46</v>
+        <v>3.4629</v>
       </c>
       <c r="D9" t="n">
-        <v>1.84</v>
+        <v>1.8444</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2.73</v>
+        <v>2.7317</v>
       </c>
       <c r="C10" t="n">
-        <v>3.22</v>
+        <v>3.2242</v>
       </c>
       <c r="D10" t="n">
-        <v>1.44</v>
+        <v>1.4422</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>3.4</v>
+        <v>3.3949</v>
       </c>
       <c r="C11" t="n">
-        <v>3.55</v>
+        <v>3.5549</v>
       </c>
       <c r="D11" t="n">
-        <v>1.32</v>
+        <v>1.319</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3.14</v>
+        <v>3.1364</v>
       </c>
       <c r="C12" t="n">
-        <v>3.65</v>
+        <v>3.6534</v>
       </c>
       <c r="D12" t="n">
-        <v>2.27</v>
+        <v>2.2688</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>2.44</v>
+        <v>2.4364</v>
       </c>
       <c r="C13" t="n">
-        <v>2.85</v>
+        <v>2.8507</v>
       </c>
       <c r="D13" t="n">
-        <v>1.21</v>
+        <v>1.2094</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2.64</v>
+        <v>2.6353</v>
       </c>
       <c r="C14" t="n">
-        <v>2.8</v>
+        <v>2.7999</v>
       </c>
       <c r="D14" t="n">
-        <v>0.88</v>
+        <v>0.8816000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.66</v>
+        <v>2.659</v>
       </c>
       <c r="C15" t="n">
-        <v>2.95</v>
+        <v>2.9465</v>
       </c>
       <c r="D15" t="n">
-        <v>1.08</v>
+        <v>1.0792</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.25</v>
+        <v>2.2528</v>
       </c>
       <c r="C16" t="n">
-        <v>2.5</v>
+        <v>2.4957</v>
       </c>
       <c r="D16" t="n">
-        <v>0.86</v>
+        <v>0.8583</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.25</v>
+        <v>2.2528</v>
       </c>
       <c r="C17" t="n">
-        <v>2.5</v>
+        <v>2.4957</v>
       </c>
       <c r="D17" t="n">
-        <v>0.86</v>
+        <v>0.8583</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.66</v>
+        <v>2.659</v>
       </c>
       <c r="C18" t="n">
-        <v>2.95</v>
+        <v>2.9465</v>
       </c>
       <c r="D18" t="n">
-        <v>1.08</v>
+        <v>1.0792</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>2.64</v>
+        <v>2.6353</v>
       </c>
       <c r="C19" t="n">
-        <v>2.8</v>
+        <v>2.7999</v>
       </c>
       <c r="D19" t="n">
-        <v>0.88</v>
+        <v>0.8816000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.44</v>
+        <v>2.4364</v>
       </c>
       <c r="C20" t="n">
-        <v>2.85</v>
+        <v>2.8507</v>
       </c>
       <c r="D20" t="n">
-        <v>1.21</v>
+        <v>1.2094</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>3.14</v>
+        <v>3.1364</v>
       </c>
       <c r="C21" t="n">
-        <v>3.65</v>
+        <v>3.6534</v>
       </c>
       <c r="D21" t="n">
-        <v>2.27</v>
+        <v>2.2688</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>3.4</v>
+        <v>3.3949</v>
       </c>
       <c r="C22" t="n">
-        <v>3.55</v>
+        <v>3.5549</v>
       </c>
       <c r="D22" t="n">
-        <v>1.32</v>
+        <v>1.319</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2.73</v>
+        <v>2.7317</v>
       </c>
       <c r="C23" t="n">
-        <v>3.22</v>
+        <v>3.2242</v>
       </c>
       <c r="D23" t="n">
-        <v>1.44</v>
+        <v>1.4422</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2.98</v>
+        <v>2.9765</v>
       </c>
       <c r="C24" t="n">
-        <v>3.46</v>
+        <v>3.4629</v>
       </c>
       <c r="D24" t="n">
-        <v>1.84</v>
+        <v>1.8444</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.19</v>
+        <v>3.1895</v>
       </c>
       <c r="C25" t="n">
-        <v>3.47</v>
+        <v>3.4672</v>
       </c>
       <c r="D25" t="n">
-        <v>1.52</v>
+        <v>1.5194</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2.85</v>
+        <v>2.8501</v>
       </c>
       <c r="C26" t="n">
-        <v>3.32</v>
+        <v>3.3194</v>
       </c>
       <c r="D26" t="n">
-        <v>1.53</v>
+        <v>1.5275</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.04</v>
+        <v>3.045</v>
       </c>
       <c r="C27" t="n">
-        <v>3.66</v>
+        <v>3.6609</v>
       </c>
       <c r="D27" t="n">
-        <v>1.83</v>
+        <v>1.8298</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3.02</v>
+        <v>3.0174</v>
       </c>
       <c r="C28" t="n">
-        <v>3.38</v>
+        <v>3.382</v>
       </c>
       <c r="D28" t="n">
-        <v>1.56</v>
+        <v>1.5601</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>3.4</v>
+        <v>3.4021</v>
       </c>
       <c r="C29" t="n">
-        <v>3.93</v>
+        <v>3.9344</v>
       </c>
       <c r="D29" t="n">
-        <v>1.55</v>
+        <v>1.5457</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>3.29</v>
+        <v>3.2872</v>
       </c>
       <c r="C30" t="n">
-        <v>3.88</v>
+        <v>3.8755</v>
       </c>
       <c r="D30" t="n">
-        <v>1.83</v>
+        <v>1.8316</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>4.02</v>
+        <v>4.0204</v>
       </c>
       <c r="C31" t="n">
-        <v>4.52</v>
+        <v>4.5157</v>
       </c>
       <c r="D31" t="n">
-        <v>1.61</v>
+        <v>1.6098</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>4.49</v>
+        <v>4.4896</v>
       </c>
       <c r="C32" t="n">
-        <v>4.11</v>
+        <v>4.1077</v>
       </c>
       <c r="D32" t="n">
-        <v>15.7</v>
+        <v>15.7036</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>4.94</v>
+        <v>4.939</v>
       </c>
       <c r="C33" t="n">
-        <v>3.91</v>
+        <v>3.9113</v>
       </c>
       <c r="D33" t="n">
-        <v>14.81</v>
+        <v>14.8169</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>42</v>
       </c>
       <c r="B34" t="n">
-        <v>4.38</v>
+        <v>4.3764</v>
       </c>
       <c r="C34" t="n">
-        <v>4.01</v>
+        <v>4.0127</v>
       </c>
       <c r="D34" t="n">
-        <v>11.53</v>
+        <v>11.5296</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>4.29</v>
+        <v>4.2893</v>
       </c>
       <c r="C35" t="n">
-        <v>4.5</v>
+        <v>4.5044</v>
       </c>
       <c r="D35" t="n">
-        <v>17.41</v>
+        <v>17.4173</v>
       </c>
     </row>
     <row r="36">
@@ -936,13 +936,13 @@
         <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>4.09</v>
+        <v>4.0908</v>
       </c>
       <c r="C36" t="n">
-        <v>4.28</v>
+        <v>4.2797</v>
       </c>
       <c r="D36" t="n">
-        <v>12.27</v>
+        <v>12.2723</v>
       </c>
     </row>
     <row r="37">
@@ -950,13 +950,13 @@
         <v>45</v>
       </c>
       <c r="B37" t="n">
-        <v>4.09</v>
+        <v>4.0948</v>
       </c>
       <c r="C37" t="n">
-        <v>4.29</v>
+        <v>4.2905</v>
       </c>
       <c r="D37" t="n">
-        <v>9.83</v>
+        <v>9.832599999999999</v>
       </c>
     </row>
     <row r="38">
@@ -964,13 +964,13 @@
         <v>46</v>
       </c>
       <c r="B38" t="n">
-        <v>4.28</v>
+        <v>4.2827</v>
       </c>
       <c r="C38" t="n">
-        <v>4.53</v>
+        <v>4.5327</v>
       </c>
       <c r="D38" t="n">
-        <v>17.2</v>
+        <v>17.2035</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>47</v>
       </c>
       <c r="B39" t="n">
-        <v>4.16</v>
+        <v>4.1559</v>
       </c>
       <c r="C39" t="n">
-        <v>4.41</v>
+        <v>4.4095</v>
       </c>
       <c r="D39" t="n">
-        <v>12.47</v>
+        <v>12.4676</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>48</v>
       </c>
       <c r="B40" t="n">
-        <v>4.09</v>
+        <v>4.0943</v>
       </c>
       <c r="C40" t="n">
-        <v>4.32</v>
+        <v>4.3221</v>
       </c>
       <c r="D40" t="n">
-        <v>9.890000000000001</v>
+        <v>9.8894</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>49</v>
       </c>
       <c r="B41" t="n">
-        <v>5.02</v>
+        <v>5.0227</v>
       </c>
       <c r="C41" t="n">
-        <v>5.34</v>
+        <v>5.3436</v>
       </c>
       <c r="D41" t="n">
-        <v>12.86</v>
+        <v>12.8589</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>4.2</v>
+        <v>4.1972</v>
       </c>
       <c r="C42" t="n">
-        <v>4.42</v>
+        <v>4.4192</v>
       </c>
       <c r="D42" t="n">
-        <v>12.59</v>
+        <v>12.5915</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>3.6</v>
+        <v>3.6008</v>
       </c>
       <c r="C43" t="n">
-        <v>3.76</v>
+        <v>3.7628</v>
       </c>
       <c r="D43" t="n">
-        <v>4.22</v>
+        <v>4.2247</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>52</v>
       </c>
       <c r="B44" t="n">
-        <v>4.2</v>
+        <v>4.2025</v>
       </c>
       <c r="C44" t="n">
-        <v>4.42</v>
+        <v>4.4195</v>
       </c>
       <c r="D44" t="n">
-        <v>12.61</v>
+        <v>12.6076</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>53</v>
       </c>
       <c r="B45" t="n">
-        <v>4.2</v>
+        <v>4.2019</v>
       </c>
       <c r="C45" t="n">
-        <v>4.42</v>
+        <v>4.4162</v>
       </c>
       <c r="D45" t="n">
-        <v>12.61</v>
+        <v>12.6058</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>54</v>
       </c>
       <c r="B46" t="n">
-        <v>4.2</v>
+        <v>4.2025</v>
       </c>
       <c r="C46" t="n">
-        <v>4.42</v>
+        <v>4.4195</v>
       </c>
       <c r="D46" t="n">
-        <v>12.61</v>
+        <v>12.6076</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>55</v>
       </c>
       <c r="B47" t="n">
-        <v>3.6</v>
+        <v>3.6008</v>
       </c>
       <c r="C47" t="n">
-        <v>3.76</v>
+        <v>3.7628</v>
       </c>
       <c r="D47" t="n">
-        <v>4.22</v>
+        <v>4.2247</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>56</v>
       </c>
       <c r="B48" t="n">
-        <v>4.2</v>
+        <v>4.1972</v>
       </c>
       <c r="C48" t="n">
-        <v>4.42</v>
+        <v>4.4192</v>
       </c>
       <c r="D48" t="n">
-        <v>12.59</v>
+        <v>12.5915</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>57</v>
       </c>
       <c r="B49" t="n">
-        <v>5.02</v>
+        <v>5.0227</v>
       </c>
       <c r="C49" t="n">
-        <v>5.34</v>
+        <v>5.3436</v>
       </c>
       <c r="D49" t="n">
-        <v>12.86</v>
+        <v>12.8589</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>58</v>
       </c>
       <c r="B50" t="n">
-        <v>4.09</v>
+        <v>4.0943</v>
       </c>
       <c r="C50" t="n">
-        <v>4.32</v>
+        <v>4.3221</v>
       </c>
       <c r="D50" t="n">
-        <v>9.890000000000001</v>
+        <v>9.8894</v>
       </c>
     </row>
     <row r="51">
@@ -1146,13 +1146,13 @@
         <v>59</v>
       </c>
       <c r="B51" t="n">
-        <v>4.16</v>
+        <v>4.1559</v>
       </c>
       <c r="C51" t="n">
-        <v>4.41</v>
+        <v>4.4095</v>
       </c>
       <c r="D51" t="n">
-        <v>12.47</v>
+        <v>12.4676</v>
       </c>
     </row>
     <row r="52">
@@ -1160,13 +1160,13 @@
         <v>60</v>
       </c>
       <c r="B52" t="n">
-        <v>4.28</v>
+        <v>4.2827</v>
       </c>
       <c r="C52" t="n">
-        <v>4.53</v>
+        <v>4.5327</v>
       </c>
       <c r="D52" t="n">
-        <v>17.2</v>
+        <v>17.2035</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>61</v>
       </c>
       <c r="B53" t="n">
-        <v>4.09</v>
+        <v>4.0948</v>
       </c>
       <c r="C53" t="n">
-        <v>4.29</v>
+        <v>4.2905</v>
       </c>
       <c r="D53" t="n">
-        <v>9.83</v>
+        <v>9.832599999999999</v>
       </c>
     </row>
     <row r="54">
@@ -1188,13 +1188,13 @@
         <v>62</v>
       </c>
       <c r="B54" t="n">
-        <v>4.09</v>
+        <v>4.0908</v>
       </c>
       <c r="C54" t="n">
-        <v>4.28</v>
+        <v>4.2797</v>
       </c>
       <c r="D54" t="n">
-        <v>12.27</v>
+        <v>12.2723</v>
       </c>
     </row>
     <row r="55">
@@ -1202,13 +1202,13 @@
         <v>63</v>
       </c>
       <c r="B55" t="n">
-        <v>4.29</v>
+        <v>4.2893</v>
       </c>
       <c r="C55" t="n">
-        <v>4.5</v>
+        <v>4.5044</v>
       </c>
       <c r="D55" t="n">
-        <v>17.41</v>
+        <v>17.4173</v>
       </c>
     </row>
     <row r="56">
@@ -1216,13 +1216,13 @@
         <v>64</v>
       </c>
       <c r="B56" t="n">
-        <v>4.38</v>
+        <v>4.3764</v>
       </c>
       <c r="C56" t="n">
-        <v>4.01</v>
+        <v>4.0127</v>
       </c>
       <c r="D56" t="n">
-        <v>11.53</v>
+        <v>11.5296</v>
       </c>
     </row>
     <row r="57">
@@ -1230,13 +1230,13 @@
         <v>65</v>
       </c>
       <c r="B57" t="n">
-        <v>4.94</v>
+        <v>4.939</v>
       </c>
       <c r="C57" t="n">
-        <v>3.91</v>
+        <v>3.9113</v>
       </c>
       <c r="D57" t="n">
-        <v>14.81</v>
+        <v>14.8169</v>
       </c>
     </row>
     <row r="58">
@@ -1244,13 +1244,13 @@
         <v>66</v>
       </c>
       <c r="B58" t="n">
-        <v>4.49</v>
+        <v>4.4896</v>
       </c>
       <c r="C58" t="n">
-        <v>4.11</v>
+        <v>4.1077</v>
       </c>
       <c r="D58" t="n">
-        <v>15.7</v>
+        <v>15.7036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>